<commit_message>
changes required for schnell added
</commit_message>
<xml_diff>
--- a/apps/web-society/src/assets/templates/vehicleBulkUpload.xlsx
+++ b/apps/web-society/src/assets/templates/vehicleBulkUpload.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PPCRC Project\fnt-flsy\apps\web-society\src\assets\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\workstation_fountlab\fnt-flsy\apps\web-society\src\assets\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E78B86-8077-445E-88DD-0CE36FDD9B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9264"/>
+    <workbookView xWindow="6720" yWindow="4935" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Building Name</t>
   </si>
@@ -30,25 +31,28 @@
     <t>Flat Number</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>Card Number</t>
   </si>
   <si>
     <t>Card Type</t>
+  </si>
+  <si>
+    <t>Vehicle Make</t>
+  </si>
+  <si>
+    <t>Vehicle Number</t>
+  </si>
+  <si>
+    <t>Vehicle Type</t>
+  </si>
+  <si>
+    <t>Device Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -111,7 +115,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -122,7 +126,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -427,24 +430,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="26" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="26" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -455,21 +458,23 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1"/>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -488,7 +493,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -516,7 +521,7 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -544,7 +549,7 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
-    <row r="4" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>

</xml_diff>